<commit_message>
Added 123 in cell A2
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22512"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9898207A-A521-4C81-BFEA-AB5098ADD7A3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F455E0B-69C0-4E64-825C-71433AC338EB}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,9 +371,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -382,7 +384,153 @@
         <v>123</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E6379276E67864F8E0EF61591E7D829" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="72c019b1667232c30679e4bb1d51d166">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a8898fd043fd830b20f0b6098ebec22">
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all/>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0710AA2-18C5-4B8B-A4AF-F076651DD08C}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBF8C576-5559-471A-9FBD-B139727F117F}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9E75372-F332-4B82-8F6E-F18D3AC0FACF}"/>
 </file>
</xml_diff>